<commit_message>
CAN1-61 #fixed issues in fifo_testcases by Waseem
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/FIFO_Test_Cases.xlsx
+++ b/Documentations/Test Cases/FIFO_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\Can_Controller\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AFEBC5-B1EB-4145-85A4-D5DE81A31309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D114F6AB-1945-494D-B79E-0F5D1B6A48B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -224,80 +224,98 @@
     <t>Write pointer gets incremented on rising edge of clock if 'i_w_en' is set to 1 and fifo is not full</t>
   </si>
   <si>
+    <t>o_full' = 1 when fifo is full</t>
+  </si>
+  <si>
+    <t>o_fifo_w_data' is saved in the fifo cell where the write pointer is pointing to at rising edge of clock if 'i_w_en' is set to 1 and fifo is not full</t>
+  </si>
+  <si>
+    <t>Read pointer gets incremented on rising edge of clock if 'i_r_en' is set to 1 and fifo is not empty</t>
+  </si>
+  <si>
+    <t>Read pointer is incremented on rising edge of clock when fifo is not empty and 'i_r_en' is set to 1</t>
+  </si>
+  <si>
+    <t>Write pointer is incremented on rising edge of clock when fifo is not full and 'i_w_en' is set to 1</t>
+  </si>
+  <si>
+    <t>o_fifo_r_data' is set to the fifo cell content where the read pointer is pointing to</t>
+  </si>
+  <si>
+    <t>All fifo cells are set to zeros when 'i_reset' is set to 1</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset' to 1
+2. Check that all fifo cells contain zeros</t>
+  </si>
+  <si>
+    <t>All fifo cells are equal to zeros</t>
+  </si>
+  <si>
+    <t>The fifo has a parameter 'DEPTH' that decides the depth of the fifo</t>
+  </si>
+  <si>
+    <t>1. Instantiate multiple FIFOs each with a different depth
+2. Observe and check that each FIFO's depth is equal to its depth parameter</t>
+  </si>
+  <si>
+    <t>DEPTH = 2, 4, 8, 16, 32 ,64</t>
+  </si>
+  <si>
+    <t>FIFO's depth is equal to the depth parameter</t>
+  </si>
+  <si>
+    <t>1. Set 'i_reset' to 1
+2. Set 'i_w_en' to 0
+3. Set 'i_r_en' to 0
+4. Set 'i_reset' to 0 after two clock cycles
+5. Check that the write pointer doen'st get incremented on the rising edge of the clock for two clock cycles
+6. set 'i_w_en' to 1
+7. Check that the write pointer gets incremented on the rising edge of the clock
+8. wait until 'o_full' is set to 1
+9. Check that the write pointer doesn't get incremented on rising edge of the clock</t>
+  </si>
+  <si>
+    <t>FIFO cell where write pointer is pointing to is equal to 128'h5 at rising edge of the clock when 'i_w_en' is set to 1 and fifo is not full</t>
+  </si>
+  <si>
     <t>1. Set 'i_reset' to 1
 2. Set 'i_w_en' to 1
-3. Set 'i_r_en' to 0
-4. Set 'i_reset' to 0 after two clock cycles
-5. Check that the write pointer gets incremented on the rising edge of the clock
-6. wait until 'o_full' is set to 1
-7. Check that the write pointer doesn't get incremented on rising edge of the clock</t>
-  </si>
-  <si>
-    <t>o_full' = 1 when fifo is full</t>
-  </si>
-  <si>
-    <t>o_fifo_w_data' is saved in the fifo cell where the write pointer is pointing to at rising edge of clock if 'i_w_en' is set to 1 and fifo is not full</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset' to 1
-2. Set 'i_w_en' to 1
-3. Set 'i_r_en' to 0
-4. Set 'i_reset' to 0 after two clock cycles
-5. Check that fifo cell where the write pointer is pointing to is equal to 'i_fifo_w_data' at rising edge of clock</t>
-  </si>
-  <si>
-    <t>Read pointer gets incremented on rising edge of clock if 'i_r_en' is set to 1 and fifo is not empty</t>
+3. Set 'i_fifo_w_data' to 128'h5 (value chosen arbitrarily)
+4. Set 'i_r_en' to 0
+5. Set 'i_reset' to 0 after two clock cycles
+6. Check that fifo cell where the write pointer is pointing to is equal to 128'h5 at rising edge of clock</t>
   </si>
   <si>
     <t>1. Set 'i_w_en' to 0
-2. Set 'i_r_en' to 1
-3. Check that the read pointer gets incremented on the rising edge of the clock
-4. wait until 'o_empty' is set to 1
-5. Check that the read pointer doesn't get incremented on rising edge of the clock</t>
-  </si>
-  <si>
-    <t>Read pointer is incremented on rising edge of clock when fifo is not empty and 'i_r_en' is set to 1</t>
-  </si>
-  <si>
-    <t>FIFO cell where write pointer is pointing to is equal to 'i_fifo_w_data' at rising edge of the clock when 'i_w_en' is set to 1 and fifo is not full</t>
-  </si>
-  <si>
-    <t>Write pointer is incremented on rising edge of clock when fifo is not full and 'i_w_en' is set to 1</t>
-  </si>
-  <si>
-    <t>o_fifo_r_data' is set to the fifo cell content where the read pointer is pointing to</t>
+2. Set 'i_r_en' to 0
+3. Check that the read pointer doesn't get incremented on the rising edge of the clock for two clock cycles
+Set 'i_r_en' to 1
+4. Check that the read pointer gets incremented on the rising edge of the clock
+5. wait until 'o_empty' is set to 1
+6. Check that the read pointer doesn't get incremented on rising edge of the clock</t>
+  </si>
+  <si>
+    <t>o_fifo_r_data' is always equal to the fifo cell where the read pointer is pointing to (in this test: 128'h8)</t>
   </si>
   <si>
     <t>1. Set 'i_w_en' to 1
-2. Set 'i_r_en' to 1
-3. Check that 'o_fifo_r_data' is always equal to the fifo cell where the read pointer is pointing to</t>
+2. Set 'i_fifo_w_data' to 128'h8 (value chosen arbitrarily)
+3. Wait for one clock cycle
+4. Set 'i_r_en' to 1
+5. Check that 'o_fifo_r_data' is always equal to the fifo cell where the read pointer is pointing to (in this test: 128'h8)</t>
   </si>
   <si>
     <t>i_reset' = 0
 'i_w_en' = 1
-'i_r_en' = 1</t>
-  </si>
-  <si>
-    <t>o_fifo_r_data' is always equal to the fifo cell where the read pointer is pointing to</t>
-  </si>
-  <si>
-    <t>All fifo cells are set to zeros when 'i_reset' is set to 1</t>
-  </si>
-  <si>
-    <t>1. Set 'i_reset' to 1
-2. Check that all fifo cells contain zeros</t>
-  </si>
-  <si>
-    <t>All fifo cells are equal to zeros</t>
-  </si>
-  <si>
-    <t>The fifo has a parameter 'DEPTH' that decides the depth of the fifo</t>
-  </si>
-  <si>
-    <t>Observe and check the presence of the depth parameter</t>
-  </si>
-  <si>
-    <t>N/A</t>
+'i_r_en' = 1
+'i_fifo_w_data' = 128'h8</t>
+  </si>
+  <si>
+    <t>i_reset' = 0
+'i_w_en' = 1
+'i_r_en' = 0
+'i_fifo_w_data' = 128'h5</t>
   </si>
 </sst>
 </file>
@@ -678,7 +696,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -731,16 +749,16 @@
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
@@ -832,7 +850,7 @@
         <v>51</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4"/>
@@ -884,7 +902,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -895,19 +913,19 @@
         <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -915,22 +933,22 @@
         <v>29</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="4"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -938,22 +956,22 @@
         <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -961,16 +979,16 @@
         <v>31</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -983,16 +1001,16 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1003,21 +1021,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1163,24 +1166,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{099A5288-121E-4A14-A6B4-83046D76B9FD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1196,4 +1197,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{065C203B-187E-495A-97A5-35B3AD3DB734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA12D9B4-0AFF-4A48-8503-C4B7A72BF3AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>